<commit_message>
Requested data from mimecast, need to find a good endpoint for email reports
</commit_message>
<xml_diff>
--- a/IT Metric Dashboard Spreadsheet.xlsx
+++ b/IT Metric Dashboard Spreadsheet.xlsx
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>99.97</v>
+        <v>100</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1008,7 +1008,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>DEN-1ST-TEMP</t>
+          <t>DEN-LAB</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1138,11 +1138,11 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>66.36</v>
+        <v>62.3</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1158,11 +1158,11 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>66.08</v>
+        <v>62.02</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1318,11 +1318,11 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>66.97</v>
+        <v>62.25</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1338,11 +1338,11 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>66.95999999999999</v>
+        <v>62.3</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1378,11 +1378,11 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>66.95999999999999</v>
+        <v>62.13</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1398,11 +1398,11 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>66.97</v>
+        <v>62.28</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1418,11 +1418,11 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>66.95</v>
+        <v>62.3</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1438,11 +1438,11 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>66.97</v>
+        <v>62.3</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1458,11 +1458,11 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>66.97</v>
+        <v>62.3</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1478,11 +1478,11 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>66.97</v>
+        <v>62.29</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1498,11 +1498,11 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>66.97</v>
+        <v>62.3</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1518,11 +1518,11 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>66.97</v>
+        <v>62.3</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1538,11 +1538,11 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>66.97</v>
+        <v>62.3</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1558,11 +1558,11 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>66.95999999999999</v>
+        <v>62.29</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1578,11 +1578,11 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>66.95999999999999</v>
+        <v>62.3</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1598,11 +1598,11 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>66.95999999999999</v>
+        <v>62.29</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1618,11 +1618,11 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>66.97</v>
+        <v>62.29</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1663,22 +1663,22 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>SLA Resolution Compliance</t>
+          <t>Resolution Rate</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D2" t="n">
-        <v>73.91</v>
+        <v>80.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>